<commit_message>
issue and issue.net remediated 8.1 and 8.2
</commit_message>
<xml_diff>
--- a/Workflow.xlsx
+++ b/Workflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1820" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="-60" yWindow="2040" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1065,13 +1065,13 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="75.5" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>

</xml_diff>